<commit_message>
Added practice, added marker feedback, clean up
</commit_message>
<xml_diff>
--- a/data_raw/MSM_dict.xlsx
+++ b/data_raw/MSM_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\MSM\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19611CE9-9289-43E7-A419-894905F75E68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B781FD5-D8D0-4878-830C-D89DAE9BF1E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>de</t>
   </si>
@@ -169,13 +169,6 @@
     <t>In the following you will hear some short piano pieces. Press the space bar when you perceive a section. After listening, we will ask you how difficult you found the task and whether you liked the piece.</t>
   </si>
   <si>
-    <t xml:space="preserve">Wann immer Sie einen Abschluss oder Neubeginn hören, klicken Sie die Leertaste. Es gibt keine richtigen und falschen Antworten. Antworten Sie einfach nach Ihrem persönlichen, ersten Eindruck.
-</t>
-  </si>
-  <si>
-    <t>Whenever you hear a conclusion or new beginning, click the space bar. There are no right and wrong answers. Just answer according to your personal, first impression.</t>
-  </si>
-  <si>
     <t>THANK_YOU</t>
   </si>
   <si>
@@ -210,6 +203,24 @@
   </si>
   <si>
     <t>Welcome! \\We are happy that you take part in our study</t>
+  </si>
+  <si>
+    <t>CONTINUE_MAIN_TEST</t>
+  </si>
+  <si>
+    <t>Weiter zum Experiment.</t>
+  </si>
+  <si>
+    <t>Conitnue to the main experiment.</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS</t>
+  </si>
+  <si>
+    <t>Wann immer Sie einen Abschluss oder Neubeginn hören, drücken Sie die Leertaste. Es gibt keine richtigen und falschen Antworten. Antworten Sie einfach nach Ihrem persönlichen, ersten Eindruck.</t>
+  </si>
+  <si>
+    <t>Whenever you hear a conclusion or new beginning, press the space bar. There are no right and wrong answers. Just answer according to your personal, first impression.</t>
   </si>
 </sst>
 </file>
@@ -567,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,10 +695,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="195" x14ac:dyDescent="0.25">
@@ -702,6 +713,9 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
@@ -722,13 +736,13 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,15 +767,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -788,24 +802,35 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>53</v>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New feedback, liking/difficulty pages, next button on item page
</commit_message>
<xml_diff>
--- a/data_raw/MSM_dict.xlsx
+++ b/data_raw/MSM_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\MSM\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B781FD5-D8D0-4878-830C-D89DAE9BF1E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942CFE4E-5098-4998-A819-2D0C9E546EB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>de</t>
   </si>
@@ -141,16 +141,7 @@
     <t>LIKING_PROMPT</t>
   </si>
   <si>
-    <t>Das Stück hat mir gefallen</t>
-  </si>
-  <si>
-    <t>I liked the piece</t>
-  </si>
-  <si>
     <t>DIFFICULTY_PROMPT</t>
-  </si>
-  <si>
-    <t>Die Aufgabe war schwierig</t>
   </si>
   <si>
     <t>The task was difficult.</t>
@@ -208,12 +199,6 @@
     <t>CONTINUE_MAIN_TEST</t>
   </si>
   <si>
-    <t>Weiter zum Experiment.</t>
-  </si>
-  <si>
-    <t>Conitnue to the main experiment.</t>
-  </si>
-  <si>
     <t>INSTRUCTIONS</t>
   </si>
   <si>
@@ -221,16 +206,92 @@
   </si>
   <si>
     <t>Whenever you hear a conclusion or new beginning, press the space bar. There are no right and wrong answers. Just answer according to your personal, first impression.</t>
+  </si>
+  <si>
+    <t>Completely disagree</t>
+  </si>
+  <si>
+    <t>Strongly disagree</t>
+  </si>
+  <si>
+    <t>Disagree</t>
+  </si>
+  <si>
+    <t>Agree</t>
+  </si>
+  <si>
+    <t>Strongly agree</t>
+  </si>
+  <si>
+    <t>Completely agree</t>
+  </si>
+  <si>
+    <t>LIKERT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trifft gar nicht zu </t>
+  </si>
+  <si>
+    <t>Trifft nicht zu</t>
+  </si>
+  <si>
+    <t>Trifft eher nicht zu</t>
+  </si>
+  <si>
+    <t>Trifft eher zu</t>
+  </si>
+  <si>
+    <t>Trifft zu</t>
+  </si>
+  <si>
+    <t>Triff sehr zu</t>
+  </si>
+  <si>
+    <t>LIKERT2</t>
+  </si>
+  <si>
+    <t>LIKERT3</t>
+  </si>
+  <si>
+    <t>LIKERT4</t>
+  </si>
+  <si>
+    <t>LIKERT5</t>
+  </si>
+  <si>
+    <t>LIKERT6</t>
+  </si>
+  <si>
+    <t>Beginne mit dem Experiment.</t>
+  </si>
+  <si>
+    <t>Start to the experiment.</t>
+  </si>
+  <si>
+    <t>Das Stück hat mir gefallen.</t>
+  </si>
+  <si>
+    <t>Die Aufgabe war schwierig.</t>
+  </si>
+  <si>
+    <t>I liked the piece.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -256,13 +317,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -578,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,10 +762,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="195" x14ac:dyDescent="0.25">
@@ -706,21 +773,21 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -736,13 +803,13 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,71 +834,161 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="2" t="s">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="B22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Wider buttons, removeEventListener to finished_page
</commit_message>
<xml_diff>
--- a/data_raw/MSM_dict.xlsx
+++ b/data_raw/MSM_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\MSM\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410DC191-733F-4539-A18B-E1EEF161821F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C257BD0-3412-4E68-B2B5-E2FC2842182F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
@@ -252,12 +252,6 @@
     <t>LIKERT6</t>
   </si>
   <si>
-    <t>Beginne mit dem Experiment.</t>
-  </si>
-  <si>
-    <t>Start to the experiment.</t>
-  </si>
-  <si>
     <t>Das Stück hat mir gefallen.</t>
   </si>
   <si>
@@ -282,16 +276,7 @@
     <t>NUM_LIKERT5</t>
   </si>
   <si>
-    <t>6 Triff sehr zu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Trifft gar nicht zu </t>
-  </si>
-  <si>
     <t>6 Completely agree</t>
-  </si>
-  <si>
-    <t>1 Completely disagree</t>
   </si>
   <si>
     <t>In the following you will hear  {{stimulus_description}}. Press the space bar when you perceive a section. After listening, we will ask you how difficult you found the task and whether you liked the piece.</t>
@@ -328,10 +313,25 @@
 </t>
   </si>
   <si>
-    <t>John Knowles Paine: Symphonie Nr. 1 in c-Moll, Op. 23: Allegro con brio. Aus der Aufnahme New World Records #80374-2. &lt;br/&gt; &amp;copy; 1989 Anthology of Recorded Music, Inc. Gebrauch mit freundlicher Genehmigung.</t>
-  </si>
-  <si>
-    <t>John Knowles Paine: Symphony No. 1 in C minor, Op. 23: Allegro con brio. From the sound recording New World Records #80374-2.  &lt;br/&gt; &amp;copy; 1989 Anthology of Recorded Music, Inc. Used by permission.</t>
+    <t>John Knowles Paine: Symphony No. 1 in C minor, Op. 23: Allegro con brio. From the sound recording New World Records #80374-2.  &lt;br/&gt; &amp;copy;1989 Anthology of Recorded Music, Inc. Used by permission.</t>
+  </si>
+  <si>
+    <t>John Knowles Paine: Symphonie Nr. 1 in c-Moll, Op. 23: Allegro con brio. Aus der Aufnahme New World Records #80374-2. &lt;br/&gt; &amp;copy;1989 Anthology of Recorded Music, Inc. Gebrauch mit freundlicher Genehmigung.</t>
+  </si>
+  <si>
+    <t>Beginne mit dem Experiment. &lt;br&gt; Viel Vergnügen!</t>
+  </si>
+  <si>
+    <t>Begin the experiment. &lt;br&gt; Have fun!</t>
+  </si>
+  <si>
+    <t>Trifft gar nicht zu 1</t>
+  </si>
+  <si>
+    <t>6 Trifft sehr zu</t>
+  </si>
+  <si>
+    <t>Completely disagree 1</t>
   </si>
 </sst>
 </file>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +837,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>40</v>
@@ -848,10 +848,10 @@
         <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,10 +914,10 @@
         <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -925,7 +925,7 @@
         <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>39</v>
@@ -958,10 +958,10 @@
         <v>53</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1056,18 +1056,18 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B30" s="3">
         <v>2</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B31" s="3">
         <v>3</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B32" s="3">
         <v>4</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B33" s="3">
         <v>5</v>
@@ -1111,46 +1111,46 @@
     </row>
     <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaning up event listeners, additional finished pages. Button widths.
</commit_message>
<xml_diff>
--- a/data_raw/MSM_dict.xlsx
+++ b/data_raw/MSM_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\MSM\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C257BD0-3412-4E68-B2B5-E2FC2842182F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B262608-5685-4C6D-AA6D-06A7853B68F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t>de</t>
   </si>
@@ -332,6 +332,24 @@
   </si>
   <si>
     <t>Completely disagree 1</t>
+  </si>
+  <si>
+    <t>FINISHED</t>
+  </si>
+  <si>
+    <t>Sie haben die Segmentierungsaufgabe beendet.</t>
+  </si>
+  <si>
+    <t>FINISHED_CONT</t>
+  </si>
+  <si>
+    <t>Sie haben die Segmentierungsaufgabe beendet. &lt;br&gt; Jetzt folgen noch ein paar weitere Fragen.</t>
+  </si>
+  <si>
+    <t>You finished the segmentation task.</t>
+  </si>
+  <si>
+    <t>You finished the segmentation task. &lt;br&gt;  Now on to a few more questions.</t>
   </si>
 </sst>
 </file>
@@ -709,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,6 +1171,28 @@
         <v>95</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed training section to only one new stimulus.
</commit_message>
<xml_diff>
--- a/data_raw/MSM_dict.xlsx
+++ b/data_raw/MSM_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lea.fink/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\MSM\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3A91AB-4BED-3941-996C-AC6C3880AE7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFAB1F0-15D4-41D1-8491-7C4DBA93C111}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8920" yWindow="500" windowWidth="29060" windowHeight="22900" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
   <sheets>
     <sheet name="HLT_dict" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
   <si>
     <t>de</t>
   </si>
@@ -336,57 +336,61 @@
     <t>In dieser Studie untersuchen wir, wie Hörerinnen und Hörer Abschnitte in der Musik wahrnehmen. Musik lässt sich in viele unterschiedliche Abschnitte gliedern: kurze und längere, deutliche und weniger deutliche. Wenn etwas neues beginnt oder etwas endet, markiert dies einen solchen Abschnitt. Was für Sie als Abschnitt zählt und was nicht, entscheiden allein Sie. Es geht nicht darum, alle Abschnitte zu finden - das wäre während des Hörens gar nicht möglich. Uns interessiert, wie Sie die Musik ganz spontan in sinnvolle Teile gliedern. Entscheiden Sie intuitiv.</t>
   </si>
   <si>
+    <t>ein Musikstück (7min)</t>
+  </si>
+  <si>
+    <t>Urheberechtshinweis</t>
+  </si>
+  <si>
+    <t>Sie hörten einige der folgende Choräle von Johann Sebastian Bach (original oder manipuliert)</t>
+  </si>
+  <si>
+    <t>Sie haben die Aufgabe beendet.</t>
+  </si>
+  <si>
+    <t>Sie haben die Aufgabe beendet. &lt;br&gt; Jetzt folgen noch ein paar weitere Fragen.</t>
+  </si>
+  <si>
+    <t>You finished the task.</t>
+  </si>
+  <si>
+    <t>You finished the task. &lt;br&gt;  Now on to a few more questions.</t>
+  </si>
+  <si>
+    <t>Beginnen Sie mit dem Experiment. &lt;br&gt; Viel Vergnügen!</t>
+  </si>
+  <si>
+    <t>a piece of music (7min)</t>
+  </si>
+  <si>
+    <t>In this study, we investigate how listeners perceive sections in music. Music can be divided into many different sections: shorter and longer, clear and less clear. A section is, for example, marked when something new begins or something ends. What counts as a section and what does not, you yourself can decide. The aim is not to identify all sections - this would not be possible while listening. We are interested in how you spontaneously divide the music into meaningful parts. Simply decide intuitively.</t>
+  </si>
+  <si>
+    <t>EXAMPLE_HEADER_PLAIN</t>
+  </si>
+  <si>
+    <t>Klicken Sie auf das Symbol, um das Stück abzuspielen. Wann immer für Sie ein Abschnitt beginnt oder endet, drücken Sie eine beliebige Taste.  Antworten Sie einfach nach Ihrem persönlichen, ersten Eindruck.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Im folgenden hören Sie  {{stimulus_description}}. Drücken Sie </t>
+      <t xml:space="preserve">Click on the button to play the audio. Whenever you hear a section concluding or beginning, press </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri (Textkörper)"/>
       </rPr>
-      <t>eine beliebige Taste</t>
+      <t>any key</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, wenn Sie einen Abschnitt wahrnehmen. Nach dem Hören fragen wir Sie, wie schwer Ihnen die Aufgabe fiel und ob Ihnen das Stück gefallen hat.</t>
+      <t>. Simply answer according to your first impressions.</t>
     </r>
-  </si>
-  <si>
-    <t>ein Musikstück (7min)</t>
-  </si>
-  <si>
-    <t>Urheberechtshinweis</t>
-  </si>
-  <si>
-    <t>Sie hörten einige der folgende Choräle von Johann Sebastian Bach (original oder manipuliert)</t>
-  </si>
-  <si>
-    <t>Sie haben die Aufgabe beendet.</t>
-  </si>
-  <si>
-    <t>Sie haben die Aufgabe beendet. &lt;br&gt; Jetzt folgen noch ein paar weitere Fragen.</t>
-  </si>
-  <si>
-    <t>You finished the task.</t>
-  </si>
-  <si>
-    <t>You finished the task. &lt;br&gt;  Now on to a few more questions.</t>
-  </si>
-  <si>
-    <t>Beginnen Sie mit dem Experiment. &lt;br&gt; Viel Vergnügen!</t>
-  </si>
-  <si>
-    <t>a piece of music (7min)</t>
-  </si>
-  <si>
-    <t>In this study, we investigate how listeners perceive sections in music. Music can be divided into many different sections: shorter and longer, clear and less clear. A section is, for example, marked when something new begins or something ends. What counts as a section and what does not, you yourself can decide. The aim is not to identify all sections - this would not be possible while listening. We are interested in how you spontaneously divide the music into meaningful parts. Simply decide intuitively.</t>
   </si>
   <si>
     <r>
@@ -396,7 +400,9 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Textkörper)"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">any key </t>
     </r>
@@ -412,72 +418,20 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Click on the button to play the audio. Whenever you hear a section concluding or beginning, press </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Textkörper)"/>
-      </rPr>
-      <t>any key</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Simply answer according to your first impressions.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Textkörper)"/>
-      </rPr>
-      <t>Klicken Sie auf das Symbol, um das Stück abzuspielen.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Wann immer für Sie ein Abschnitt beginnt oder endet, drücken Sie</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Textkörper)"/>
-      </rPr>
-      <t xml:space="preserve"> eine beliebige Taste</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.  Antworten Sie einfach nach Ihrem persönlichen, ersten Eindruck.</t>
-    </r>
+    <t>Im folgenden hören Sie  {{stimulus_description}}. Drücken Sie eine beliebige Taste, wenn Sie einen Abschnitt wahrnehmen. Nach dem Hören fragen wir Sie, wie schwer Ihnen die Aufgabe fiel und ob Ihnen das Stück gefallen hat.</t>
+  </si>
+  <si>
+    <t>Ein Beispiel</t>
+  </si>
+  <si>
+    <t>An Example</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,19 +454,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Textkörper)"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri (Textkörper)"/>
     </font>
   </fonts>
@@ -536,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -562,6 +516,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -876,20 +833,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="78.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="65.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="78.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -900,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -911,7 +868,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -922,7 +879,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -933,7 +890,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -944,7 +901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -955,7 +912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -966,7 +923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -977,7 +934,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -988,7 +945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -999,7 +956,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="120">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1007,21 +964,21 @@
         <v>101</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1032,346 +989,357 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:7" ht="45">
+      <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B18" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:7">
+      <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:7">
+      <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    <row r="23" spans="1:7">
+      <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:7" ht="15.75">
+      <c r="A24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75">
+      <c r="A30" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:7" ht="15.75">
+      <c r="A31" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B31" s="6">
         <v>2</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C31" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:7" ht="15.75">
+      <c r="A32" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B32" s="6">
         <v>3</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C32" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:3" ht="15.75">
+      <c r="A33" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B33" s="6">
         <v>4</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C33" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:3" ht="15.75">
+      <c r="A34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B34" s="6">
         <v>5</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C34" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="35" spans="1:3" ht="15.75">
+      <c r="A35" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:3">
+      <c r="A42" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B42" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C42" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+    <row r="43" spans="1:3" ht="15.75">
+      <c r="A43" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B43" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C43" s="10" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change instructions, practice now for PART2 as well, without practic item.
</commit_message>
<xml_diff>
--- a/data_raw/MSM_dict.xlsx
+++ b/data_raw/MSM_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\MSM\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFAB1F0-15D4-41D1-8491-7C4DBA93C111}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFFAF81-D7DE-4826-A7A8-965CD6A14E03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3CDF385B-FF42-4ECC-9678-5E042E73A117}"/>
   </bookViews>
   <sheets>
     <sheet name="HLT_dict" sheetId="1" r:id="rId1"/>
@@ -279,12 +279,6 @@
     <t>PART1_STIMULUS_DESCRIPTION</t>
   </si>
   <si>
-    <t>einige kurze Klavierstücke</t>
-  </si>
-  <si>
-    <t>some short piano pieces</t>
-  </si>
-  <si>
     <t>PART2_STIMULUS_DESCRIPTION</t>
   </si>
   <si>
@@ -294,9 +288,6 @@
     <t>John Knowles Paine: Symphonie Nr. 1 in c-Moll, Op. 23: Allegro con brio. Aus der Aufnahme New World Records #80374-2. &lt;br/&gt; &amp;copy;1989 Anthology of Recorded Music, Inc. Gebrauch mit freundlicher Genehmigung.</t>
   </si>
   <si>
-    <t>Begin the experiment. &lt;br&gt; Have fun!</t>
-  </si>
-  <si>
     <t>6 Trifft sehr zu</t>
   </si>
   <si>
@@ -355,9 +346,6 @@
   </si>
   <si>
     <t>You finished the task. &lt;br&gt;  Now on to a few more questions.</t>
-  </si>
-  <si>
-    <t>Beginnen Sie mit dem Experiment. &lt;br&gt; Viel Vergnügen!</t>
   </si>
   <si>
     <t>a piece of music (7min)</t>
@@ -425,6 +413,18 @@
   </si>
   <si>
     <t>An Example</t>
+  </si>
+  <si>
+    <t>Jetzt beginnt das Experiment. &lt;br&gt; Viel Vergnügen!</t>
+  </si>
+  <si>
+    <t>Now the experiment starts. &lt;br&gt; Have fun!</t>
+  </si>
+  <si>
+    <t>{{num_items}} kurze Klavierstücke</t>
+  </si>
+  <si>
+    <t>{{num_items}} piano pieces</t>
   </si>
 </sst>
 </file>
@@ -835,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68BC7805-D1BA-4C3B-8218-2DF65AF09233}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -961,10 +961,10 @@
         <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45">
@@ -972,10 +972,10 @@
         <v>53</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -991,13 +991,13 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1038,10 +1038,10 @@
         <v>45</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1093,10 +1093,10 @@
         <v>52</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75">
@@ -1194,10 +1194,10 @@
         <v>75</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75">
@@ -1249,7 +1249,7 @@
         <v>81</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>80</v>
@@ -1260,87 +1260,87 @@
         <v>82</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75">
       <c r="A43" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>